<commit_message>
setting up for review in future
</commit_message>
<xml_diff>
--- a/Median of Two Sorted Arrays/Whiteboards/Solution.xlsx
+++ b/Median of Two Sorted Arrays/Whiteboards/Solution.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\Median of Two Sorted Arrays\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD298D9-DD92-4E77-B7BE-8F87C4B95D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE28C98A-94CD-4889-98FF-B603F594FC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{F2127D3C-7F13-43C5-B155-16DA742AA00A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{F2127D3C-7F13-43C5-B155-16DA742AA00A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1 (1.5)" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet6" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet7" sheetId="9" r:id="rId6"/>
+    <sheet name="5" sheetId="5" r:id="rId4"/>
+    <sheet name="6" sheetId="7" r:id="rId5"/>
+    <sheet name="7" sheetId="9" r:id="rId6"/>
+    <sheet name="8" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="104">
   <si>
     <t>up</t>
   </si>
@@ -369,6 +370,12 @@
   <si>
     <t>median is half of 550+480 = 515</t>
   </si>
+  <si>
+    <t>continuing here with thinking about edge cases</t>
+  </si>
+  <si>
+    <t>look at 7 first for review</t>
+  </si>
 </sst>
 </file>
 
@@ -512,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -610,6 +617,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -13203,8 +13213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F03A608-D9BB-4045-B439-7D147A8A887F}">
   <dimension ref="A2:AT96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AS89" sqref="AS89"/>
+    <sheetView topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Z73" sqref="Z73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15656,4 +15666,305 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17A57DD-EF5C-47BF-83FA-9065E32E78A7}">
+  <dimension ref="D2:AH9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AL11" sqref="AL11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="4:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16">
+        <v>0</v>
+      </c>
+      <c r="I2" s="16">
+        <v>1</v>
+      </c>
+      <c r="J2" s="16">
+        <v>2</v>
+      </c>
+      <c r="K2" s="16">
+        <v>3</v>
+      </c>
+      <c r="L2" s="16">
+        <v>4</v>
+      </c>
+      <c r="M2" s="16">
+        <v>5</v>
+      </c>
+      <c r="N2" s="16">
+        <v>6</v>
+      </c>
+      <c r="O2" s="16">
+        <v>7</v>
+      </c>
+      <c r="P2" s="16">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="16">
+        <v>9</v>
+      </c>
+      <c r="R2" s="16">
+        <v>10</v>
+      </c>
+      <c r="S2" s="16">
+        <v>11</v>
+      </c>
+      <c r="T2" s="16">
+        <v>12</v>
+      </c>
+      <c r="U2" s="16">
+        <v>13</v>
+      </c>
+      <c r="V2" s="16">
+        <v>14</v>
+      </c>
+      <c r="W2" s="16">
+        <v>15</v>
+      </c>
+      <c r="X2" s="16">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="16">
+        <v>17</v>
+      </c>
+      <c r="Z2" s="16">
+        <v>18</v>
+      </c>
+      <c r="AA2" s="16">
+        <v>19</v>
+      </c>
+      <c r="AB2" s="16">
+        <v>20</v>
+      </c>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG2" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH2" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="4:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="35">
+        <v>1</v>
+      </c>
+      <c r="I3" s="35">
+        <v>100</v>
+      </c>
+      <c r="J3" s="35">
+        <v>200</v>
+      </c>
+      <c r="K3" s="35">
+        <v>300</v>
+      </c>
+      <c r="L3" s="35">
+        <v>400</v>
+      </c>
+      <c r="M3" s="35">
+        <v>450</v>
+      </c>
+      <c r="N3" s="35">
+        <v>460</v>
+      </c>
+      <c r="O3" s="35">
+        <v>470</v>
+      </c>
+      <c r="P3" s="35">
+        <v>480</v>
+      </c>
+      <c r="Q3" s="35">
+        <v>550</v>
+      </c>
+      <c r="R3" s="35">
+        <v>660</v>
+      </c>
+      <c r="S3" s="35">
+        <v>670</v>
+      </c>
+      <c r="T3" s="35">
+        <v>680</v>
+      </c>
+      <c r="U3" s="35">
+        <v>690</v>
+      </c>
+      <c r="V3" s="35">
+        <v>700</v>
+      </c>
+      <c r="W3" s="35">
+        <v>710</v>
+      </c>
+      <c r="X3" s="35">
+        <v>720</v>
+      </c>
+      <c r="Y3" s="35">
+        <v>800</v>
+      </c>
+      <c r="Z3" s="35">
+        <v>900</v>
+      </c>
+      <c r="AA3" s="35">
+        <v>950</v>
+      </c>
+      <c r="AB3" s="35">
+        <v>999</v>
+      </c>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16">
+        <v>20</v>
+      </c>
+      <c r="AG3" s="16">
+        <v>20</v>
+      </c>
+      <c r="AH3" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="4:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="35">
+        <v>0</v>
+      </c>
+      <c r="I4" s="35">
+        <v>50</v>
+      </c>
+      <c r="J4" s="35">
+        <v>100</v>
+      </c>
+      <c r="K4" s="35">
+        <v>100</v>
+      </c>
+      <c r="L4" s="35">
+        <v>100</v>
+      </c>
+      <c r="M4" s="35">
+        <v>400</v>
+      </c>
+      <c r="N4" s="35">
+        <v>400</v>
+      </c>
+      <c r="O4" s="35">
+        <v>400</v>
+      </c>
+      <c r="P4" s="35">
+        <v>400</v>
+      </c>
+      <c r="Q4" s="35">
+        <v>400</v>
+      </c>
+      <c r="R4" s="35">
+        <v>660</v>
+      </c>
+      <c r="S4" s="35">
+        <v>888</v>
+      </c>
+      <c r="T4" s="35">
+        <v>888</v>
+      </c>
+      <c r="U4" s="35">
+        <v>888</v>
+      </c>
+      <c r="V4" s="35">
+        <v>888</v>
+      </c>
+      <c r="W4" s="35">
+        <v>888</v>
+      </c>
+      <c r="X4" s="35">
+        <v>888</v>
+      </c>
+      <c r="Y4" s="35">
+        <v>888</v>
+      </c>
+      <c r="Z4" s="35">
+        <v>889</v>
+      </c>
+      <c r="AA4" s="35">
+        <v>900</v>
+      </c>
+      <c r="AB4" s="35">
+        <v>950</v>
+      </c>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="16"/>
+    </row>
+    <row r="5" spans="4:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="16"/>
+      <c r="AH5" s="16"/>
+    </row>
+    <row r="8" spans="4:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="4:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>